<commit_message>
fix: add my_codes.py to .gitignore to prevent tracking of local code files
</commit_message>
<xml_diff>
--- a/data/input/data_ground_truth_01/legenda.xlsx
+++ b/data/input/data_ground_truth_01/legenda.xlsx
@@ -286,7 +286,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="20:25"/>
+      <selection pane="bottomLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -459,7 +459,7 @@
         <v>0.16</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2</v>

</xml_diff>